<commit_message>
fix location stage quest name
</commit_message>
<xml_diff>
--- a/GameInformation/game-info.xlsx
+++ b/GameInformation/game-info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan\OneDrive\Počítač\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programing\java\street-of-code\assignment\gladiatus\GameInformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78F98C5-C049-44BB-B57B-AD7CB43864F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C934CE66-7A12-4606-BE7D-CB314920642C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D80F13DF-F1D4-4D07-A3F0-527E13F812A1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
   <si>
     <t>COMMON</t>
   </si>
@@ -247,9 +247,6 @@
   </si>
   <si>
     <t>without elite and boss</t>
-  </si>
-  <si>
-    <t>heruwmafmuzew</t>
   </si>
   <si>
     <t>Bear Cave</t>
@@ -553,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -629,8 +626,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -947,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2472DD-865D-4C96-B099-508B86271E7A}">
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,7 +1599,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" s="16">
         <v>1</v>
@@ -1677,7 +1672,7 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" s="16">
         <v>2</v>
@@ -2497,17 +2492,17 @@
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="47">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" s="47">
+      <c r="C46">
         <v>1300</v>
       </c>
     </row>
@@ -2547,14 +2542,14 @@
         <v>1</v>
       </c>
       <c r="D60">
-        <f>E19</f>
+        <f t="shared" ref="D60:D69" si="16">E19</f>
         <v>2</v>
       </c>
       <c r="E60" t="s">
         <v>71</v>
       </c>
       <c r="F60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="3:8" x14ac:dyDescent="0.25">
@@ -2562,7 +2557,7 @@
         <v>2</v>
       </c>
       <c r="D61">
-        <f>E20</f>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
       <c r="E61" t="s">
@@ -2572,7 +2567,7 @@
         <v>72</v>
       </c>
       <c r="G61" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.25">
@@ -2580,7 +2575,7 @@
         <v>3</v>
       </c>
       <c r="D62">
-        <f>E21</f>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
     </row>
@@ -2589,7 +2584,7 @@
         <v>4</v>
       </c>
       <c r="D63">
-        <f>E22</f>
+        <f t="shared" si="16"/>
         <v>3</v>
       </c>
     </row>
@@ -2598,7 +2593,7 @@
         <v>5</v>
       </c>
       <c r="D64">
-        <f>E23</f>
+        <f t="shared" si="16"/>
         <v>4</v>
       </c>
     </row>
@@ -2607,7 +2602,7 @@
         <v>6</v>
       </c>
       <c r="D65">
-        <f>E24</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
@@ -2616,7 +2611,7 @@
         <v>7</v>
       </c>
       <c r="D66">
-        <f>E25</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
@@ -2625,7 +2620,7 @@
         <v>8</v>
       </c>
       <c r="D67">
-        <f>E26</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
@@ -2634,7 +2629,7 @@
         <v>9</v>
       </c>
       <c r="D68">
-        <f>E27</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
     </row>
@@ -2643,16 +2638,13 @@
         <v>10</v>
       </c>
       <c r="D69">
-        <f>E28</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="3:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C70" s="37">
         <v>1</v>
-      </c>
-      <c r="D70" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="71" spans="3:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add new region, locations and related items
</commit_message>
<xml_diff>
--- a/GameInformation/game-info.xlsx
+++ b/GameInformation/game-info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programing\java\street-of-code\assignment\gladiatus\GameInformation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C934CE66-7A12-4606-BE7D-CB314920642C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2056E16-6105-44F5-B85F-12EB657BA4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D80F13DF-F1D4-4D07-A3F0-527E13F812A1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="81">
   <si>
     <t>COMMON</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>UsableQuestItem</t>
+  </si>
+  <si>
+    <t>ADDITIONAL</t>
+  </si>
+  <si>
+    <t>Tranquil Gardens</t>
   </si>
 </sst>
 </file>
@@ -942,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2472DD-865D-4C96-B099-508B86271E7A}">
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,6 +1018,9 @@
       <c r="H3" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="I3" t="s">
+        <v>79</v>
+      </c>
       <c r="L3" s="44" t="s">
         <v>8</v>
       </c>
@@ -1158,24 +1167,27 @@
         <v>53</v>
       </c>
       <c r="D7" s="11">
-        <f t="shared" ref="D7:D14" si="4">C7*$D$4</f>
-        <v>21.200000000000003</v>
+        <f>C7*$D$4+I7</f>
+        <v>26.200000000000003</v>
       </c>
       <c r="E7" s="11">
-        <f t="shared" si="0"/>
-        <v>34.450000000000003</v>
+        <f>C7*$E$4+I7</f>
+        <v>39.450000000000003</v>
       </c>
       <c r="F7" s="11">
-        <f t="shared" si="1"/>
-        <v>47.7</v>
+        <f>C7*$F$4+I7</f>
+        <v>52.7</v>
       </c>
       <c r="G7" s="11">
-        <f t="shared" si="2"/>
-        <v>63.599999999999994</v>
+        <f>C7*$G$4+I7</f>
+        <v>68.599999999999994</v>
       </c>
       <c r="H7" s="15">
-        <f t="shared" si="3"/>
-        <v>74.199999999999989</v>
+        <f>C7*$H$4+I7</f>
+        <v>79.199999999999989</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
       </c>
       <c r="K7">
         <v>3</v>
@@ -1202,8 +1214,8 @@
         <v>67</v>
       </c>
       <c r="D8" s="11">
-        <f t="shared" si="4"/>
-        <v>26.8</v>
+        <f t="shared" ref="D8:D14" si="4">C8*$D$4+I8</f>
+        <v>33.799999999999997</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="0"/>
@@ -1218,8 +1230,11 @@
         <v>80.399999999999991</v>
       </c>
       <c r="H8" s="15">
-        <f t="shared" si="3"/>
-        <v>93.8</v>
+        <f t="shared" ref="H8:H14" si="5">C8*$H$4+I8</f>
+        <v>100.8</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
       </c>
       <c r="K8">
         <v>4</v>
@@ -1247,7 +1262,7 @@
       </c>
       <c r="D9" s="11">
         <f t="shared" si="4"/>
-        <v>32.4</v>
+        <v>41.4</v>
       </c>
       <c r="E9" s="11">
         <f t="shared" si="0"/>
@@ -1262,8 +1277,11 @@
         <v>97.2</v>
       </c>
       <c r="H9" s="15">
-        <f t="shared" si="3"/>
-        <v>113.39999999999999</v>
+        <f t="shared" si="5"/>
+        <v>122.39999999999999</v>
+      </c>
+      <c r="I9">
+        <v>9</v>
       </c>
       <c r="K9">
         <v>5</v>
@@ -1290,8 +1308,8 @@
         <v>95</v>
       </c>
       <c r="D10" s="11">
-        <f t="shared" si="4"/>
-        <v>38</v>
+        <f>C10*$D$4+I10</f>
+        <v>49</v>
       </c>
       <c r="E10" s="11">
         <f t="shared" si="0"/>
@@ -1306,8 +1324,11 @@
         <v>114</v>
       </c>
       <c r="H10" s="15">
-        <f t="shared" si="3"/>
-        <v>133</v>
+        <f t="shared" si="5"/>
+        <v>144</v>
+      </c>
+      <c r="I10">
+        <v>11</v>
       </c>
       <c r="K10">
         <v>6</v>
@@ -1335,7 +1356,7 @@
       </c>
       <c r="D11" s="11">
         <f t="shared" si="4"/>
-        <v>43.6</v>
+        <v>56.6</v>
       </c>
       <c r="E11" s="11">
         <f t="shared" si="0"/>
@@ -1350,8 +1371,11 @@
         <v>130.79999999999998</v>
       </c>
       <c r="H11" s="15">
-        <f t="shared" si="3"/>
-        <v>152.6</v>
+        <f t="shared" si="5"/>
+        <v>165.6</v>
+      </c>
+      <c r="I11">
+        <v>13</v>
       </c>
       <c r="K11">
         <v>7</v>
@@ -1379,7 +1403,7 @@
       </c>
       <c r="D12" s="11">
         <f t="shared" si="4"/>
-        <v>49.2</v>
+        <v>64.2</v>
       </c>
       <c r="E12" s="11">
         <f t="shared" si="0"/>
@@ -1394,8 +1418,11 @@
         <v>147.6</v>
       </c>
       <c r="H12" s="15">
-        <f t="shared" si="3"/>
-        <v>172.2</v>
+        <f t="shared" si="5"/>
+        <v>187.2</v>
+      </c>
+      <c r="I12">
+        <v>15</v>
       </c>
       <c r="K12">
         <v>8</v>
@@ -1423,7 +1450,7 @@
       </c>
       <c r="D13" s="11">
         <f t="shared" si="4"/>
-        <v>54.800000000000004</v>
+        <v>71.800000000000011</v>
       </c>
       <c r="E13" s="11">
         <f t="shared" si="0"/>
@@ -1438,8 +1465,11 @@
         <v>164.4</v>
       </c>
       <c r="H13" s="15">
-        <f t="shared" si="3"/>
-        <v>191.79999999999998</v>
+        <f t="shared" si="5"/>
+        <v>208.79999999999998</v>
+      </c>
+      <c r="I13">
+        <v>17</v>
       </c>
       <c r="K13">
         <v>9</v>
@@ -1466,8 +1496,8 @@
         <v>151</v>
       </c>
       <c r="D14" s="11">
-        <f t="shared" si="4"/>
-        <v>60.400000000000006</v>
+        <f>C14*$D$4+I14</f>
+        <v>79.400000000000006</v>
       </c>
       <c r="E14" s="11">
         <f t="shared" si="0"/>
@@ -1482,8 +1512,11 @@
         <v>181.2</v>
       </c>
       <c r="H14" s="15">
-        <f t="shared" si="3"/>
-        <v>211.39999999999998</v>
+        <f t="shared" si="5"/>
+        <v>230.39999999999998</v>
+      </c>
+      <c r="I14">
+        <v>19</v>
       </c>
       <c r="K14">
         <v>10</v>
@@ -1681,7 +1714,7 @@
         <v>3</v>
       </c>
       <c r="D20">
-        <f t="shared" ref="D20:D27" si="5">P20 * C20</f>
+        <f t="shared" ref="D20:D27" si="6">P20 * C20</f>
         <v>780</v>
       </c>
       <c r="E20">
@@ -1695,7 +1728,7 @@
         <v>16</v>
       </c>
       <c r="H20">
-        <f t="shared" ref="H20:H27" si="6" xml:space="preserve"> $H$17*E20</f>
+        <f t="shared" ref="H20:H27" si="7" xml:space="preserve"> $H$17*E20</f>
         <v>150</v>
       </c>
       <c r="I20">
@@ -1705,11 +1738,11 @@
         <v>0</v>
       </c>
       <c r="K20">
-        <f t="shared" ref="K20:K27" si="7">I20 * U20</f>
+        <f t="shared" ref="K20:K27" si="8">I20 * U20</f>
         <v>76</v>
       </c>
       <c r="L20" s="17">
-        <f t="shared" ref="L20:L27" si="8">J20*V20</f>
+        <f t="shared" ref="L20:L27" si="9">J20*V20</f>
         <v>0</v>
       </c>
       <c r="M20" s="27">
@@ -1727,19 +1760,19 @@
         <v>260</v>
       </c>
       <c r="S20">
-        <f t="shared" ref="S20:S27" si="9">B6 * 13 + $S$17</f>
+        <f t="shared" ref="S20:S27" si="10">B6 * 13 + $S$17</f>
         <v>36</v>
       </c>
       <c r="T20">
-        <f t="shared" ref="T20:T27" si="10">B6 * 13 + $T$17</f>
+        <f t="shared" ref="T20:T27" si="11">B6 * 13 + $T$17</f>
         <v>51</v>
       </c>
       <c r="U20">
-        <f t="shared" ref="U20:U27" si="11">B6 * 13 + $U$17</f>
+        <f t="shared" ref="U20:U27" si="12">B6 * 13 + $U$17</f>
         <v>76</v>
       </c>
       <c r="V20" s="17">
-        <f t="shared" ref="V20:V27" si="12">B6 * 13 + $V$17</f>
+        <f t="shared" ref="V20:V27" si="13">B6 * 13 + $V$17</f>
         <v>126</v>
       </c>
     </row>
@@ -1751,22 +1784,22 @@
         <v>3</v>
       </c>
       <c r="D21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1020</v>
       </c>
       <c r="E21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21:F27" si="13">G21 * S21</f>
-        <v>833</v>
+        <f t="shared" ref="F21:F27" si="14">G21 * S21</f>
+        <v>931</v>
       </c>
       <c r="G21">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H21">
-        <f t="shared" si="6"/>
-        <v>150</v>
+        <f t="shared" si="7"/>
+        <v>200</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -1775,19 +1808,19 @@
         <v>0</v>
       </c>
       <c r="K21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>178</v>
       </c>
       <c r="L21" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M21" s="27">
-        <f t="shared" ref="M21:M27" si="14">D21+F21 + H21 + K21 + L21</f>
-        <v>2181</v>
+        <f t="shared" ref="M21:M27" si="15">D21+F21 + H21 + K21 + L21</f>
+        <v>2329</v>
       </c>
       <c r="N21" s="25">
-        <f t="shared" ref="N21:N27" si="15">$N$17 * B7 * O21</f>
+        <f t="shared" ref="N21:N27" si="16">$N$17 * B7 * O21</f>
         <v>2700</v>
       </c>
       <c r="O21">
@@ -1797,19 +1830,19 @@
         <v>340</v>
       </c>
       <c r="S21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>49</v>
       </c>
       <c r="T21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>64</v>
       </c>
       <c r="U21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>89</v>
       </c>
       <c r="V21" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>139</v>
       </c>
     </row>
@@ -1821,21 +1854,21 @@
         <v>3</v>
       </c>
       <c r="D22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1260</v>
       </c>
       <c r="E22">
         <v>3</v>
       </c>
       <c r="F22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1116</v>
       </c>
       <c r="G22">
         <v>18</v>
       </c>
       <c r="H22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>150</v>
       </c>
       <c r="I22">
@@ -1845,19 +1878,19 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>204</v>
       </c>
       <c r="L22" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M22" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2730</v>
       </c>
       <c r="N22" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3900</v>
       </c>
       <c r="O22">
@@ -1867,19 +1900,19 @@
         <v>420</v>
       </c>
       <c r="S22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>62</v>
       </c>
       <c r="T22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>77</v>
       </c>
       <c r="U22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>102</v>
       </c>
       <c r="V22" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>152</v>
       </c>
     </row>
@@ -1891,21 +1924,21 @@
         <v>3</v>
       </c>
       <c r="D23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1500</v>
       </c>
       <c r="E23">
         <v>4</v>
       </c>
       <c r="F23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1650</v>
       </c>
       <c r="G23">
         <v>22</v>
       </c>
       <c r="H23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>200</v>
       </c>
       <c r="I23">
@@ -1915,19 +1948,19 @@
         <v>1</v>
       </c>
       <c r="K23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>230</v>
       </c>
       <c r="L23" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>165</v>
       </c>
       <c r="M23" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3745</v>
       </c>
       <c r="N23" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5250</v>
       </c>
       <c r="O23">
@@ -1937,19 +1970,19 @@
         <v>500</v>
       </c>
       <c r="S23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>75</v>
       </c>
       <c r="T23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>90</v>
       </c>
       <c r="U23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>115</v>
       </c>
       <c r="V23" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>165</v>
       </c>
     </row>
@@ -1961,21 +1994,21 @@
         <v>3</v>
       </c>
       <c r="D24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1740</v>
       </c>
       <c r="E24">
         <v>2</v>
       </c>
       <c r="F24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1144</v>
       </c>
       <c r="G24">
         <v>13</v>
       </c>
       <c r="H24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="I24">
@@ -1985,19 +2018,19 @@
         <v>1</v>
       </c>
       <c r="K24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>384</v>
       </c>
       <c r="L24" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>178</v>
       </c>
       <c r="M24" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>3546</v>
       </c>
       <c r="N24" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>6750</v>
       </c>
       <c r="O24">
@@ -2007,19 +2040,19 @@
         <v>580</v>
       </c>
       <c r="S24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>88</v>
       </c>
       <c r="T24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>103</v>
       </c>
       <c r="U24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>128</v>
       </c>
       <c r="V24" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>178</v>
       </c>
     </row>
@@ -2031,21 +2064,21 @@
         <v>3</v>
       </c>
       <c r="D25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1980</v>
       </c>
       <c r="E25">
         <v>2</v>
       </c>
       <c r="F25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1313</v>
       </c>
       <c r="G25">
         <v>13</v>
       </c>
       <c r="H25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="I25">
@@ -2055,19 +2088,19 @@
         <v>2</v>
       </c>
       <c r="K25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>564</v>
       </c>
       <c r="L25" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>382</v>
       </c>
       <c r="M25" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4339</v>
       </c>
       <c r="N25" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8400</v>
       </c>
       <c r="O25">
@@ -2077,19 +2110,19 @@
         <v>660</v>
       </c>
       <c r="S25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>101</v>
       </c>
       <c r="T25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>116</v>
       </c>
       <c r="U25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>141</v>
       </c>
       <c r="V25" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>191</v>
       </c>
     </row>
@@ -2101,21 +2134,21 @@
         <v>4</v>
       </c>
       <c r="D26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2960</v>
       </c>
       <c r="E26">
         <v>2</v>
       </c>
       <c r="F26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1596</v>
       </c>
       <c r="G26">
         <v>14</v>
       </c>
       <c r="H26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="I26">
@@ -2125,19 +2158,19 @@
         <v>2</v>
       </c>
       <c r="K26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>616</v>
       </c>
       <c r="L26" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>408</v>
       </c>
       <c r="M26" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5680</v>
       </c>
       <c r="N26" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>10200</v>
       </c>
       <c r="O26">
@@ -2147,19 +2180,19 @@
         <v>740</v>
       </c>
       <c r="S26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>114</v>
       </c>
       <c r="T26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>129</v>
       </c>
       <c r="U26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>154</v>
       </c>
       <c r="V26" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>204</v>
       </c>
     </row>
@@ -2171,21 +2204,21 @@
         <v>4</v>
       </c>
       <c r="D27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3280</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1905</v>
       </c>
       <c r="G27">
         <v>15</v>
       </c>
       <c r="H27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="I27">
@@ -2195,19 +2228,19 @@
         <v>2</v>
       </c>
       <c r="K27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1002</v>
       </c>
       <c r="L27" s="17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>434</v>
       </c>
       <c r="M27" s="27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>6721</v>
       </c>
       <c r="N27" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>12150</v>
       </c>
       <c r="O27">
@@ -2217,19 +2250,19 @@
         <v>820</v>
       </c>
       <c r="S27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>127</v>
       </c>
       <c r="T27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>142</v>
       </c>
       <c r="U27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>167</v>
       </c>
       <c r="V27" s="17">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>217</v>
       </c>
     </row>
@@ -2542,7 +2575,7 @@
         <v>1</v>
       </c>
       <c r="D60">
-        <f t="shared" ref="D60:D69" si="16">E19</f>
+        <f t="shared" ref="D60:D69" si="17">E19</f>
         <v>2</v>
       </c>
       <c r="E60" t="s">
@@ -2557,7 +2590,7 @@
         <v>2</v>
       </c>
       <c r="D61">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3</v>
       </c>
       <c r="E61" t="s">
@@ -2575,8 +2608,11 @@
         <v>3</v>
       </c>
       <c r="D62">
-        <f t="shared" si="16"/>
-        <v>3</v>
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="E62" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.25">
@@ -2584,7 +2620,7 @@
         <v>4</v>
       </c>
       <c r="D63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3</v>
       </c>
     </row>
@@ -2593,7 +2629,7 @@
         <v>5</v>
       </c>
       <c r="D64">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
     </row>
@@ -2602,7 +2638,7 @@
         <v>6</v>
       </c>
       <c r="D65">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
     </row>
@@ -2611,7 +2647,7 @@
         <v>7</v>
       </c>
       <c r="D66">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
     </row>
@@ -2620,7 +2656,7 @@
         <v>8</v>
       </c>
       <c r="D67">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
     </row>
@@ -2629,7 +2665,7 @@
         <v>9</v>
       </c>
       <c r="D68">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
     </row>
@@ -2638,7 +2674,7 @@
         <v>10</v>
       </c>
       <c r="D69">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>